<commit_message>
Graphics Lab 2 및 수업
</commit_message>
<xml_diff>
--- a/FileStructure/UpdateAlgorithm/UpdateAlogrithm.xlsx
+++ b/FileStructure/UpdateAlgorithm/UpdateAlogrithm.xlsx
@@ -9,14 +9,13 @@
   <sheets>
     <sheet name="Transaction" sheetId="1" r:id="rId1"/>
     <sheet name="OldMaster" sheetId="2" r:id="rId2"/>
-    <sheet name="NewMaster" r:id="rId6" sheetId="3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="42">
   <si>
     <t>D</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -184,98 +183,13 @@
   <si>
     <t>U</t>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>KEY</t>
-  </si>
-  <si>
-    <t>FIRST_NAME</t>
-  </si>
-  <si>
-    <t>FAMILY_NAME</t>
-  </si>
-  <si>
-    <t>AGE</t>
-  </si>
-  <si>
-    <t>Dorothy</t>
-  </si>
-  <si>
-    <t>Kwon</t>
-  </si>
-  <si>
-    <t>Margarida</t>
-  </si>
-  <si>
-    <t>Myung</t>
-  </si>
-  <si>
-    <t>Martina</t>
-  </si>
-  <si>
-    <t>Kim</t>
-  </si>
-  <si>
-    <t>Michel</t>
-  </si>
-  <si>
-    <t>Yoo</t>
-  </si>
-  <si>
-    <t>Francis</t>
-  </si>
-  <si>
-    <t>Van</t>
-  </si>
-  <si>
-    <t>Lucy</t>
-  </si>
-  <si>
-    <t>Ryu</t>
-  </si>
-  <si>
-    <t>Floerence</t>
-  </si>
-  <si>
-    <t>La</t>
-  </si>
-  <si>
-    <t>Cordelia</t>
-  </si>
-  <si>
-    <t>Na</t>
-  </si>
-  <si>
-    <t>Aliean</t>
-  </si>
-  <si>
-    <t>Hong</t>
-  </si>
-  <si>
-    <t>Angela</t>
-  </si>
-  <si>
-    <t>Seo</t>
-  </si>
-  <si>
-    <t>Aileen</t>
-  </si>
-  <si>
-    <t>Lee</t>
-  </si>
-  <si>
-    <t>Jammy</t>
-  </si>
-  <si>
-    <t>Kan</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -627,10 +541,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="4.625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.25" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="14.125" collapsed="true"/>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="4.625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.25" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -771,14 +685,14 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="4.625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="12.25" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="14.125" collapsed="true"/>
+    <col min="1" max="1" width="4.625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.25" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -972,209 +886,4 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D2" t="n">
-        <v>14.0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D3" t="n">
-        <v>20.0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="B4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D4" t="n">
-        <v>23.0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="B5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C5" t="s">
-        <v>53</v>
-      </c>
-      <c r="D5" t="n">
-        <v>50.0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>6.0</v>
-      </c>
-      <c r="B6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C6" t="s">
-        <v>55</v>
-      </c>
-      <c r="D6" t="n">
-        <v>25.0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>7.0</v>
-      </c>
-      <c r="B7" t="s">
-        <v>56</v>
-      </c>
-      <c r="C7" t="s">
-        <v>57</v>
-      </c>
-      <c r="D7" t="n">
-        <v>42.0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="B8" t="s">
-        <v>58</v>
-      </c>
-      <c r="C8" t="s">
-        <v>59</v>
-      </c>
-      <c r="D8" t="n">
-        <v>31.0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>9.0</v>
-      </c>
-      <c r="B9" t="s">
-        <v>60</v>
-      </c>
-      <c r="C9" t="s">
-        <v>61</v>
-      </c>
-      <c r="D9" t="n">
-        <v>21.0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>10.0</v>
-      </c>
-      <c r="B10" t="s">
-        <v>62</v>
-      </c>
-      <c r="C10" t="s">
-        <v>63</v>
-      </c>
-      <c r="D10" t="n">
-        <v>22.0</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>11.0</v>
-      </c>
-      <c r="B11" t="s">
-        <v>64</v>
-      </c>
-      <c r="C11" t="s">
-        <v>65</v>
-      </c>
-      <c r="D11" t="n">
-        <v>10.0</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>12.0</v>
-      </c>
-      <c r="B12" t="s">
-        <v>66</v>
-      </c>
-      <c r="C12" t="s">
-        <v>67</v>
-      </c>
-      <c r="D12" t="n">
-        <v>20.0</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>15.0</v>
-      </c>
-      <c r="B13" t="s">
-        <v>68</v>
-      </c>
-      <c r="C13" t="s">
-        <v>69</v>
-      </c>
-      <c r="D13" t="n">
-        <v>23.0</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>20.0</v>
-      </c>
-      <c r="B14"/>
-      <c r="C14"/>
-      <c r="D14"/>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
 </file>
</xml_diff>